<commit_message>
KC Modyfikacja metody create_classes oraz dodanie kirunków studiów
</commit_message>
<xml_diff>
--- a/program_testowy.xlsx
+++ b/program_testowy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof\Desktop\Uczenie Maszynowe\class_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D70DD-7AA2-40E2-8321-2FF14BF0026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F219D5-5469-448A-8B63-762EE8462345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>nazwa_przedmiotu</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>['Agnieszka Drwalewska', 'Włodzimierz Fechner', 'Marek Galewski']</t>
+  </si>
+  <si>
+    <t>kierunek</t>
+  </si>
+  <si>
+    <t>matematyka stosowana</t>
   </si>
 </sst>
 </file>
@@ -156,12 +162,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -291,20 +300,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -326,8 +338,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -349,8 +364,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -372,8 +390,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -395,8 +416,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -418,8 +442,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -440,6 +467,9 @@
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st test of random schedule passed
</commit_message>
<xml_diff>
--- a/program_testowy.xlsx
+++ b/program_testowy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof\Desktop\Uczenie Maszynowe\class_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D70DD-7AA2-40E2-8321-2FF14BF0026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F219D5-5469-448A-8B63-762EE8462345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>nazwa_przedmiotu</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>['Agnieszka Drwalewska', 'Włodzimierz Fechner', 'Marek Galewski']</t>
+  </si>
+  <si>
+    <t>kierunek</t>
+  </si>
+  <si>
+    <t>matematyka stosowana</t>
   </si>
 </sst>
 </file>
@@ -156,12 +162,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -291,20 +300,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="61.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -326,8 +338,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -349,8 +364,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -372,8 +390,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -395,8 +416,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -418,8 +442,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -440,6 +467,9 @@
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>